<commit_message>
Adding user sample data
</commit_message>
<xml_diff>
--- a/EntityMapping.xlsx
+++ b/EntityMapping.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidfekke/Documents/node/projects/lcorner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/node/projects/lcorner/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="4960" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Id</t>
   </si>
@@ -121,16 +121,48 @@
   </si>
   <si>
     <t>Filename</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>c7f5a5a8-6648-443d-b8cf-490efc32adb6</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>jsmith@yahoo.com</t>
+  </si>
+  <si>
+    <t>904-555-9273</t>
+  </si>
+  <si>
+    <t>ashid7hdeaip78ai</t>
+  </si>
+  <si>
+    <t>30f8c3e1-0186-4330-8d4c-0b1ed44cc403</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,13 +185,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,137 +471,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="2">
+        <v>42719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="2">
+        <v>42719</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -573,7 +652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -581,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -589,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -604,10 +683,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,15 +694,18 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -631,7 +713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -639,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -647,7 +729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -655,7 +737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -663,7 +745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -678,23 +760,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -702,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -710,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -725,23 +810,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -757,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -765,7 +853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>

</xml_diff>